<commit_message>
Termino da seção 3 e inicio da 4
</commit_message>
<xml_diff>
--- a/Secao03/Exercicios_Excel_Intermadiário.xlsx
+++ b/Secao03/Exercicios_Excel_Intermadiário.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\gabrielrstan\Aulas\Curso_de_Excel_do_Basico_ao_Avancado_Macro_e_VBA_plus_Power_BI\Secao03\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="375" windowWidth="23250" windowHeight="12450" tabRatio="903" firstSheet="7" activeTab="11"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="20595" windowHeight="45" tabRatio="903" firstSheet="10" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Professor ARRUMAR" sheetId="8" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="139">
   <si>
     <t>rose@gmail.com</t>
   </si>
@@ -683,9 +683,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -874,7 +874,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -891,7 +891,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -920,7 +920,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="6" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -933,8 +933,8 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Moeda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1259,25 +1259,25 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="52.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.75" style="1"/>
-    <col min="5" max="5" width="52.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="1"/>
+    <col min="5" max="5" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="27">
+    <row r="2" spans="2:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="s">
         <v>77</v>
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="2:16">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="2:16" ht="25.5">
+    <row r="4" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
         <v>76</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="2:16" ht="25.5">
+    <row r="5" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B5" s="2" t="s">
         <v>82</v>
       </c>
@@ -1297,17 +1297,17 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="2:16" ht="25.5">
+    <row r="6" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B6" s="2"/>
       <c r="E6" s="2"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="2:16" ht="25.5">
+    <row r="7" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B7" s="2"/>
       <c r="E7" s="2"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="2:16" ht="19.5">
+    <row r="8" spans="2:16" ht="21" x14ac:dyDescent="0.35">
       <c r="B8" s="15" t="s">
         <v>74</v>
       </c>
@@ -1319,7 +1319,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="2:16" ht="25.5">
+    <row r="9" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:16" ht="25.5">
+    <row r="10" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B10" s="7" t="s">
         <v>20</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>89.99</v>
       </c>
     </row>
-    <row r="11" spans="2:16" ht="25.5">
+    <row r="11" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B11" s="7" t="s">
         <v>21</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>69.989999999999995</v>
       </c>
     </row>
-    <row r="12" spans="2:16" ht="25.5">
+    <row r="12" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B12" s="7" t="s">
         <v>27</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>153.4</v>
       </c>
     </row>
-    <row r="13" spans="2:16" ht="25.5">
+    <row r="13" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B13" s="7" t="s">
         <v>22</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>148.56</v>
       </c>
     </row>
-    <row r="14" spans="2:16" ht="25.5">
+    <row r="14" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B14" s="7" t="s">
         <v>23</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>146.13999999999999</v>
       </c>
     </row>
-    <row r="15" spans="2:16" ht="25.5">
+    <row r="15" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B15" s="7" t="s">
         <v>24</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>224.14</v>
       </c>
     </row>
-    <row r="16" spans="2:16" ht="25.5">
+    <row r="16" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B16" s="7" t="s">
         <v>25</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>150.5</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="25.5">
+    <row r="17" spans="2:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B17" s="7" t="s">
         <v>26</v>
       </c>
@@ -1475,25 +1475,25 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="52.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.75" style="1"/>
-    <col min="5" max="5" width="52.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="1"/>
+    <col min="5" max="5" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="27">
+    <row r="2" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="s">
         <v>77</v>
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="2:10">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="2:10" ht="25.5">
+    <row r="4" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
         <v>76</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="25.5">
+    <row r="5" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B5" s="2" t="s">
         <v>82</v>
       </c>
@@ -1513,17 +1513,17 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="25.5">
+    <row r="6" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B6" s="2"/>
       <c r="E6" s="2"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="2:10" ht="25.5">
+    <row r="7" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B7" s="2"/>
       <c r="E7" s="2"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="2:10" ht="19.5">
+    <row r="8" spans="2:10" ht="21" x14ac:dyDescent="0.35">
       <c r="B8" s="15" t="s">
         <v>74</v>
       </c>
@@ -1535,7 +1535,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="2:10" ht="25.5">
+    <row r="9" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="25.5">
+    <row r="10" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B10" s="7" t="s">
         <v>78</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>89.99</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="25.5">
+    <row r="11" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B11" s="7" t="s">
         <v>79</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>69.989999999999995</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="25.5">
+    <row r="12" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B12" s="7" t="s">
         <v>80</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>153.4</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="25.5">
+    <row r="13" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B13" s="7" t="s">
         <v>81</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>148.56</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="25.5">
+    <row r="14" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B14" s="7" t="s">
         <v>28</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>146.13999999999999</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="25.5">
+    <row r="15" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B15" s="7" t="s">
         <v>29</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>224.14</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="25.5">
+    <row r="16" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B16" s="7" t="s">
         <v>30</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>150.5</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="25.5">
+    <row r="17" spans="2:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B17" s="7" t="s">
         <v>31</v>
       </c>
@@ -1691,18 +1691,18 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="52.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="13.75" style="1" customWidth="1"/>
-    <col min="7" max="7" width="29.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="13.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20">
+    <row r="1" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E1"/>
       <c r="G1"/>
     </row>
-    <row r="2" spans="2:20" ht="27">
+    <row r="2" spans="2:20" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="s">
         <v>77</v>
       </c>
@@ -1710,12 +1710,12 @@
       <c r="G2"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="2:20">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E3"/>
       <c r="G3"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="2:20" ht="25.5">
+    <row r="4" spans="2:20" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
         <v>83</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="2:20" ht="25.5">
+    <row r="5" spans="2:20" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B5" s="2"/>
       <c r="E5" s="2"/>
       <c r="G5"/>
@@ -1735,7 +1735,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="2:20" ht="25.5">
+    <row r="6" spans="2:20" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="2:20" ht="25.5">
+    <row r="7" spans="2:20" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B7" s="7" t="s">
         <v>125</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:20" ht="25.5">
+    <row r="8" spans="2:20" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B8" s="7" t="s">
         <v>126</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>5.25</v>
       </c>
     </row>
-    <row r="9" spans="2:20" ht="25.5">
+    <row r="9" spans="2:20" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B9" s="7" t="s">
         <v>127</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:20" ht="25.5">
+    <row r="10" spans="2:20" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B10" s="7" t="s">
         <v>128</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="11" spans="2:20" ht="25.5">
+    <row r="11" spans="2:20" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B11" s="7" t="s">
         <v>129</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>5.75</v>
       </c>
     </row>
-    <row r="12" spans="2:20" ht="25.5">
+    <row r="12" spans="2:20" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B12" s="7" t="s">
         <v>130</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="13" spans="2:20" ht="25.5">
+    <row r="13" spans="2:20" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B13" s="7" t="s">
         <v>131</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="2:20" ht="25.5">
+    <row r="14" spans="2:20" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B14" s="7" t="s">
         <v>132</v>
       </c>
@@ -1933,23 +1933,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D9" sqref="D9:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="56.125" style="13" customWidth="1"/>
+    <col min="2" max="3" width="56.140625" style="13" customWidth="1"/>
     <col min="4" max="4" width="48" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="2:15" ht="27">
+    <row r="2" spans="2:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="s">
         <v>77</v>
       </c>
@@ -1958,14 +1958,14 @@
       <c r="F2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="2:15">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="F3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="2:15" ht="25.5">
+    <row r="4" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
         <v>87</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="25.5">
+    <row r="5" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B5" s="2" t="s">
         <v>88</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="25.5">
+    <row r="6" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="1"/>
@@ -1999,7 +1999,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="25.5">
+    <row r="8" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B8" s="12" t="s">
         <v>12</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="25.5">
+    <row r="9" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B9" s="9" t="s">
         <v>84</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>Produto Feminino Meia</v>
       </c>
     </row>
-    <row r="10" spans="2:15" ht="25.5">
+    <row r="10" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B10" s="9" t="s">
         <v>85</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>Meia Feminina Produto</v>
       </c>
     </row>
-    <row r="11" spans="2:15" ht="25.5">
+    <row r="11" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B11" s="9" t="s">
         <v>14</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>Camisa Masculina</v>
       </c>
     </row>
-    <row r="12" spans="2:15" ht="25.5">
+    <row r="12" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B12" s="9" t="s">
         <v>15</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>Bermuda Masculino</v>
       </c>
     </row>
-    <row r="13" spans="2:15" ht="25.5">
+    <row r="13" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B13" s="9" t="s">
         <v>16</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>Camisa Masculina Festa Balada</v>
       </c>
     </row>
-    <row r="14" spans="2:15" ht="25.5">
+    <row r="14" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B14" s="9" t="s">
         <v>86</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>Produto Jogger Meia</v>
       </c>
     </row>
-    <row r="15" spans="2:15" ht="25.5">
+    <row r="15" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B15" s="9" t="s">
         <v>17</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>Jaqueta Masculina Preta</v>
       </c>
     </row>
-    <row r="16" spans="2:15" ht="25.5">
+    <row r="16" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B16" s="9" t="s">
         <v>18</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>Bolsa de Trabalho</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="25.5">
+    <row r="17" spans="2:4" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B17" s="9" t="s">
         <v>19</v>
       </c>
@@ -2137,29 +2137,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O15"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.5" style="13" customWidth="1"/>
-    <col min="8" max="8" width="55.125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="51.42578125" style="13" customWidth="1"/>
+    <col min="8" max="8" width="55.140625" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1"/>
       <c r="H1"/>
     </row>
-    <row r="2" spans="2:15" ht="27">
+    <row r="2" spans="2:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="s">
         <v>77</v>
       </c>
@@ -2169,7 +2169,7 @@
       <c r="G2"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="2:15">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="F3" s="1"/>
@@ -2179,7 +2179,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="25.5">
+    <row r="4" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
         <v>89</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="25.5">
+    <row r="5" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="1"/>
@@ -2205,7 +2205,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="25.5">
+    <row r="6" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B6" s="3" t="s">
         <v>62</v>
       </c>
@@ -2228,7 +2228,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="25.5">
+    <row r="7" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B7" s="7" t="s">
         <v>38</v>
       </c>
@@ -2238,10 +2238,16 @@
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-    </row>
-    <row r="8" spans="2:15" ht="25.5">
+      <c r="G7" s="18" t="str">
+        <f>TRIM(PROPER(B7))&amp;" "&amp; TRIM(PROPER(C7))&amp;" "&amp; TRIM(PROPER(D7))&amp;" "&amp; TRIM(PROPER(E7))&amp;" "&amp; TRIM(PROPER(F7))</f>
+        <v xml:space="preserve">Tênis Feminino   </v>
+      </c>
+      <c r="H7" s="18" t="str">
+        <f>CONCATENATE(TRIM(PROPER(B7))," ",TRIM(PROPER(C7))," ",TRIM(PROPER(D7))," ",TRIM(PROPER(E7))," ",TRIM(PROPER(F7)))</f>
+        <v xml:space="preserve">Tênis Feminino   </v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B8" s="7" t="s">
         <v>37</v>
       </c>
@@ -2253,10 +2259,16 @@
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-    </row>
-    <row r="9" spans="2:15" ht="25.5">
+      <c r="G8" s="18" t="str">
+        <f t="shared" ref="G8:G15" si="0">TRIM(PROPER(B8))&amp;" "&amp; TRIM(PROPER(C8))&amp;" "&amp; TRIM(PROPER(D8))&amp;" "&amp; TRIM(PROPER(E8))&amp;" "&amp; TRIM(PROPER(F8))</f>
+        <v xml:space="preserve">Calça Feminina Jogger  </v>
+      </c>
+      <c r="H8" s="18" t="str">
+        <f t="shared" ref="H8:H15" si="1">CONCATENATE(TRIM(PROPER(B8))," ",TRIM(PROPER(C8))," ",TRIM(PROPER(D8))," ",TRIM(PROPER(E8))," ",TRIM(PROPER(F8)))</f>
+        <v xml:space="preserve">Calça Feminina Jogger  </v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B9" s="7" t="s">
         <v>39</v>
       </c>
@@ -2266,10 +2278,16 @@
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-    </row>
-    <row r="10" spans="2:15" ht="25.5">
+      <c r="G9" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Camisa Masculina   </v>
+      </c>
+      <c r="H9" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Camisa Masculina   </v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B10" s="7" t="s">
         <v>41</v>
       </c>
@@ -2279,10 +2297,16 @@
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-    </row>
-    <row r="11" spans="2:15" ht="25.5">
+      <c r="G10" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Bermuda Masculino   </v>
+      </c>
+      <c r="H10" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Bermuda Masculino   </v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B11" s="7" t="s">
         <v>56</v>
       </c>
@@ -2296,10 +2320,16 @@
         <v>61</v>
       </c>
       <c r="F11" s="7"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-    </row>
-    <row r="12" spans="2:15" ht="25.5">
+      <c r="G11" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Camisa Masculina Festa Balada </v>
+      </c>
+      <c r="H11" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Camisa Masculina Festa Balada </v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B12" s="7" t="s">
         <v>42</v>
       </c>
@@ -2309,10 +2339,16 @@
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-    </row>
-    <row r="13" spans="2:15" ht="25.5">
+      <c r="G12" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Bota Masculina   </v>
+      </c>
+      <c r="H12" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Bota Masculina   </v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B13" s="7" t="s">
         <v>43</v>
       </c>
@@ -2324,10 +2360,16 @@
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-    </row>
-    <row r="14" spans="2:15" ht="25.5">
+      <c r="G13" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Jaqueta Masculina Preta  </v>
+      </c>
+      <c r="H13" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Jaqueta Masculina Preta  </v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B14" s="7" t="s">
         <v>45</v>
       </c>
@@ -2339,10 +2381,16 @@
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-    </row>
-    <row r="15" spans="2:15" ht="25.5">
+      <c r="G14" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Bolsa De Trabalho  </v>
+      </c>
+      <c r="H14" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Bolsa De Trabalho  </v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B15" s="7" t="s">
         <v>48</v>
       </c>
@@ -2358,8 +2406,14 @@
       <c r="F15" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
+      <c r="G15" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>Kit De Pinceis De Maquiagem</v>
+      </c>
+      <c r="H15" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>Kit De Pinceis De Maquiagem</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -2370,38 +2424,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O12"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="57.5" customWidth="1"/>
-    <col min="3" max="3" width="22.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5" customWidth="1"/>
-    <col min="7" max="7" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E1"/>
       <c r="F1" s="1"/>
       <c r="H1"/>
     </row>
-    <row r="2" spans="2:15" ht="27">
+    <row r="2" spans="2:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="s">
         <v>77</v>
       </c>
       <c r="E2"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="2:15">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E3"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="2:15" ht="25.5">
+    <row r="4" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
         <v>90</v>
       </c>
@@ -2412,7 +2466,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="25.5">
+    <row r="5" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="F5" s="1"/>
@@ -2421,7 +2475,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="25.5">
+    <row r="6" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
@@ -2444,14 +2498,26 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="25.5">
+    <row r="7" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
+      <c r="C7" s="20">
+        <f>FIND("@",B7)</f>
+        <v>5</v>
+      </c>
+      <c r="D7" s="20">
+        <f>FIND(".",B7,C7)</f>
+        <v>11</v>
+      </c>
+      <c r="E7" s="20" t="str">
+        <f>MID(B7,C7+1,D7-C7-1)</f>
+        <v>gmail</v>
+      </c>
+      <c r="F7" s="20" t="str">
+        <f>MID(B7,FIND("@",B7)+1,FIND(".",B7,C7)-FIND("@",B7)-1)</f>
+        <v>gmail</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -2459,14 +2525,26 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="25.5">
+    <row r="8" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
+      <c r="C8" s="20">
+        <f t="shared" ref="C8:C12" si="0">FIND("@",B8)</f>
+        <v>6</v>
+      </c>
+      <c r="D8" s="20">
+        <f t="shared" ref="D8:D12" si="1">FIND(".",B8,C8)</f>
+        <v>14</v>
+      </c>
+      <c r="E8" s="20" t="str">
+        <f t="shared" ref="E8:E12" si="2">MID(B8,C8+1,D8-C8-1)</f>
+        <v>hotmail</v>
+      </c>
+      <c r="F8" s="20" t="str">
+        <f t="shared" ref="F8:F12" si="3">MID(B8,FIND("@",B8)+1,FIND(".",B8,C8)-FIND("@",B8)-1)</f>
+        <v>hotmail</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -2474,47 +2552,95 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="25.5">
+    <row r="9" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
+      <c r="C9" s="20">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D9" s="20">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="E9" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>yahoo</v>
+      </c>
+      <c r="F9" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>yahoo</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="2:15" ht="25.5">
+    <row r="10" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B10" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
+      <c r="C10" s="20">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D10" s="20">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="E10" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>gmail</v>
+      </c>
+      <c r="F10" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>gmail</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="2:15" ht="25.5">
+    <row r="11" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-    </row>
-    <row r="12" spans="2:15" ht="25.5">
+      <c r="C11" s="20">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D11" s="20">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="E11" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>hotmail</v>
+      </c>
+      <c r="F11" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>hotmail</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
+      <c r="C12" s="20">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D12" s="20">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="E12" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>yahoo</v>
+      </c>
+      <c r="F12" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>yahoo</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2534,25 +2660,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O9"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="57.5" customWidth="1"/>
-    <col min="3" max="3" width="22.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="32.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F1" s="1"/>
       <c r="G1"/>
     </row>
-    <row r="2" spans="2:15" ht="27">
+    <row r="2" spans="2:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="s">
         <v>77</v>
       </c>
@@ -2560,7 +2686,7 @@
       <c r="G2"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="2:15">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F3" s="1"/>
       <c r="G3"/>
       <c r="H3" s="1"/>
@@ -2568,7 +2694,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="25.5">
+    <row r="4" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
         <v>99</v>
       </c>
@@ -2580,7 +2706,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="19.5" customHeight="1">
+    <row r="5" spans="2:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="E5" s="1"/>
@@ -2590,7 +2716,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="25.5">
+    <row r="6" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -2610,36 +2736,63 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="25.5">
+    <row r="7" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="C7" s="20">
+        <f>FIND(":",B7)</f>
+        <v>9</v>
+      </c>
+      <c r="D7" s="20" t="str">
+        <f>MID(B7,C7+1,99)</f>
+        <v xml:space="preserve"> 4554-1101</v>
+      </c>
+      <c r="E7" s="20" t="str">
+        <f>MID(B7,FIND(":",B7)+1,99)</f>
+        <v xml:space="preserve"> 4554-1101</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="O7" s="21"/>
     </row>
-    <row r="8" spans="2:15" ht="25.5">
+    <row r="8" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B8" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
+      <c r="C8" s="20">
+        <f t="shared" ref="C8:C9" si="0">FIND(":",B8)</f>
+        <v>4</v>
+      </c>
+      <c r="D8" s="20" t="str">
+        <f t="shared" ref="D8:D9" si="1">MID(B8,C8+1,99)</f>
+        <v xml:space="preserve"> 123.456.789-10</v>
+      </c>
+      <c r="E8" s="20" t="str">
+        <f t="shared" ref="E8:E9" si="2">MID(B8,FIND(":",B8)+1,99)</f>
+        <v xml:space="preserve"> 123.456.789-10</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="2:15" ht="25.5">
+    <row r="9" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B9" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
+      <c r="C9" s="20">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D9" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> 06.990.590/0001-23</v>
+      </c>
+      <c r="E9" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> 06.990.590/0001-23</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -2653,25 +2806,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P16"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="57.5" customWidth="1"/>
-    <col min="3" max="3" width="22.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="40.25" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.5" customWidth="1"/>
-    <col min="7" max="7" width="23.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.42578125" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
       <c r="F1" s="1"/>
       <c r="G1"/>
     </row>
-    <row r="2" spans="2:16" ht="27">
+    <row r="2" spans="2:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="s">
         <v>77</v>
       </c>
@@ -2679,7 +2832,7 @@
       <c r="G2"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="2:16">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="F3" s="1"/>
       <c r="G3"/>
       <c r="H3" s="1"/>
@@ -2687,7 +2840,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="25.5">
+    <row r="4" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
         <v>100</v>
       </c>
@@ -2699,7 +2852,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="2:16" ht="25.5">
+    <row r="5" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B5" s="2" t="s">
         <v>101</v>
       </c>
@@ -2711,7 +2864,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="2:16" ht="19.5" customHeight="1">
+    <row r="6" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="E6" s="1"/>
@@ -2721,7 +2874,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="25.5">
+    <row r="7" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
@@ -2746,45 +2899,75 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="2:16" ht="25.5">
+    <row r="8" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B8" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
+      <c r="C8" s="20">
+        <f>FIND(":",B8)</f>
+        <v>9</v>
+      </c>
+      <c r="D8" s="20" t="str">
+        <f>MID(B8,C8+1,1000)</f>
+        <v xml:space="preserve"> 45541101</v>
+      </c>
+      <c r="E8" s="20" t="str">
+        <f>MID(B8,FIND(":",B8)+1,1000)</f>
+        <v xml:space="preserve"> 45541101</v>
+      </c>
+      <c r="F8" s="20" t="str">
+        <f>MID(E8,1,5)&amp;"-"&amp;MID(E8,6,9)</f>
+        <v xml:space="preserve"> 4554-1101</v>
+      </c>
+      <c r="G8" s="20" t="str">
+        <f>MID(MID(B8,FIND(":",B8)+1,1000),1,5)&amp;"-"&amp;MID(MID(B8,FIND(":",B8)+1,1000),6,9)</f>
+        <v xml:space="preserve"> 4554-1101</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="P8" s="21" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="25.5">
+    <row r="9" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B9" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
+      <c r="C9" s="20">
+        <f>FIND(":",B9)</f>
+        <v>4</v>
+      </c>
+      <c r="D9" s="20" t="str">
+        <f>MID(B9,C9+1,1000)</f>
+        <v xml:space="preserve"> 12345678910</v>
+      </c>
+      <c r="E9" s="20" t="str">
+        <f>MID(B9,FIND(":",B9)+1,1000)</f>
+        <v xml:space="preserve"> 12345678910</v>
+      </c>
+      <c r="F9" s="20" t="str">
+        <f>MID(E9,1,4)&amp;"."&amp;MID(E9,5,3)&amp;"."&amp;MID(E9,8,3)&amp;"-"&amp;MID(E9,11,2)</f>
+        <v xml:space="preserve"> 123.456.789-10</v>
+      </c>
+      <c r="G9" s="20" t="str">
+        <f>MID(MID(B9,FIND(":",B9)+1,1000),1,4)&amp;"."&amp;MID(MID(B9,FIND(":",B9)+1,1000),5,3)&amp;"."&amp;MID(MID(B9,FIND(":",B9)+1,1000),8,3)&amp;"-"&amp;MID(MID(B9,FIND(":",B9)+1,1000),11,2)</f>
+        <v xml:space="preserve"> 123.456.789-10</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="P9" s="21"/>
     </row>
-    <row r="10" spans="2:16">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="P10" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="2:16" ht="25.5">
+    <row r="11" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="P11" s="21" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="2:16" ht="25.5">
+    <row r="12" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="H12" s="1"/>
@@ -2792,7 +2975,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="2:16" ht="25.5">
+    <row r="13" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B13" s="3" t="s">
         <v>9</v>
       </c>
@@ -2802,31 +2985,53 @@
       <c r="D13" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="6" t="s">
+        <v>73</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="2:16" ht="25.5">
+    <row r="14" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B14" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="1"/>
+      <c r="C14" s="20" t="str">
+        <f>LEFT(B14,3)</f>
+        <v>Tel</v>
+      </c>
+      <c r="D14" s="20" t="str">
+        <f>IF(LEFT(B14,3)="CPF","É CPF","É Telefone")</f>
+        <v>É Telefone</v>
+      </c>
+      <c r="E14" s="20" t="str">
+        <f>IF(LEFT(B14,3)="CPF",MID(MID(B14,FIND(":",B14,1)+2,1000),1,3)&amp;"."&amp;MID(MID(B14,FIND(":",B14,1)+2,1000),4,3)&amp;"."&amp;MID(MID(B14,FIND(":",B14,1)+2,1000),7,3)&amp;"-"&amp;MID(MID(B14,FIND(":",B14,1)+2,1000),10,2),
+MID(MID(B14,FIND(":",B14,1)+2,1000),1,4)&amp;"-"&amp;MID(MID(B14,FIND(":",B14,1)+2,1000),5,4))</f>
+        <v>4554-1101</v>
+      </c>
       <c r="F14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="2:16" ht="25.5">
+    <row r="15" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B15" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="1"/>
+      <c r="C15" s="20" t="str">
+        <f>LEFT(B15,3)</f>
+        <v>CPF</v>
+      </c>
+      <c r="D15" s="20" t="str">
+        <f>IF(LEFT(B15,3)="CPF","É CPF","É Telefone")</f>
+        <v>É CPF</v>
+      </c>
+      <c r="E15" s="20" t="str">
+        <f>IF(LEFT(B15,3)="CPF",MID(MID(B15,FIND(":",B15,1)+2,1000),1,3)&amp;"."&amp;MID(MID(B15,FIND(":",B15,1)+2,1000),4,3)&amp;"."&amp;MID(MID(B15,FIND(":",B15,1)+2,1000),7,3)&amp;"-"&amp;MID(MID(B15,FIND(":",B15,1)+2,1000),10,2),
+MID(MID(B15,FIND(":",B15,1)+2,1000),1,4)&amp;"-"&amp;MID(MID(B15,FIND(":",B15,1)+2,1000),5,4))</f>
+        <v>123.456.789-10</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="2:16">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="H16" s="1"/>
@@ -2844,25 +3049,25 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="52.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.75" style="1"/>
-    <col min="5" max="5" width="52.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="1"/>
+    <col min="5" max="5" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="27">
+    <row r="2" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="s">
         <v>77</v>
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="2:10">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="2:10" ht="25.5">
+    <row r="4" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
         <v>76</v>
       </c>
@@ -2872,7 +3077,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="25.5">
+    <row r="5" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B5" s="2" t="s">
         <v>82</v>
       </c>
@@ -2882,17 +3087,17 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="25.5">
+    <row r="6" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B6" s="2"/>
       <c r="E6" s="2"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="2:10" ht="25.5">
+    <row r="7" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B7" s="2"/>
       <c r="E7" s="2"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="2:10" ht="19.5">
+    <row r="8" spans="2:10" ht="21" x14ac:dyDescent="0.35">
       <c r="B8" s="15" t="s">
         <v>74</v>
       </c>
@@ -2904,7 +3109,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="2:10" ht="25.5">
+    <row r="9" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
@@ -2918,7 +3123,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="25.5">
+    <row r="10" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B10" s="7" t="s">
         <v>78</v>
       </c>
@@ -2934,7 +3139,7 @@
         <v>89.99</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="25.5">
+    <row r="11" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B11" s="7" t="s">
         <v>79</v>
       </c>
@@ -2950,7 +3155,7 @@
         <v>69.989999999999995</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="25.5">
+    <row r="12" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B12" s="7" t="s">
         <v>80</v>
       </c>
@@ -2966,7 +3171,7 @@
         <v>153.4</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="25.5">
+    <row r="13" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B13" s="7" t="s">
         <v>81</v>
       </c>
@@ -2982,7 +3187,7 @@
         <v>148.56</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="25.5">
+    <row r="14" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B14" s="7" t="s">
         <v>28</v>
       </c>
@@ -2998,7 +3203,7 @@
         <v>146.13999999999999</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="25.5">
+    <row r="15" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B15" s="7" t="s">
         <v>29</v>
       </c>
@@ -3014,7 +3219,7 @@
         <v>224.14</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="25.5">
+    <row r="16" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B16" s="7" t="s">
         <v>30</v>
       </c>
@@ -3030,7 +3235,7 @@
         <v>150.5</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="25.5">
+    <row r="17" spans="2:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B17" s="7" t="s">
         <v>31</v>
       </c>
@@ -3060,19 +3265,19 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="52.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="13.75" style="1" customWidth="1"/>
-    <col min="7" max="7" width="29.125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="32.875" customWidth="1"/>
+    <col min="2" max="2" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="13.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20">
+    <row r="1" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E1"/>
       <c r="G1"/>
     </row>
-    <row r="2" spans="2:20" ht="27">
+    <row r="2" spans="2:20" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="s">
         <v>77</v>
       </c>
@@ -3080,12 +3285,12 @@
       <c r="G2"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="2:20">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E3"/>
       <c r="G3"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="2:20" ht="25.5">
+    <row r="4" spans="2:20" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
         <v>83</v>
       </c>
@@ -3096,7 +3301,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="2:20" ht="25.5">
+    <row r="5" spans="2:20" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B5" s="2"/>
       <c r="E5" s="2"/>
       <c r="G5"/>
@@ -3105,7 +3310,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="2:20" ht="25.5">
+    <row r="6" spans="2:20" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
@@ -3128,7 +3333,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="2:20" ht="25.5">
+    <row r="7" spans="2:20" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B7" s="7" t="s">
         <v>125</v>
       </c>
@@ -3153,7 +3358,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:20" ht="25.5">
+    <row r="8" spans="2:20" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B8" s="7" t="s">
         <v>126</v>
       </c>
@@ -3178,7 +3383,7 @@
         <v>5.25</v>
       </c>
     </row>
-    <row r="9" spans="2:20" ht="25.5">
+    <row r="9" spans="2:20" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B9" s="7" t="s">
         <v>127</v>
       </c>
@@ -3203,7 +3408,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:20" ht="25.5">
+    <row r="10" spans="2:20" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B10" s="7" t="s">
         <v>128</v>
       </c>
@@ -3228,7 +3433,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="11" spans="2:20" ht="25.5">
+    <row r="11" spans="2:20" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B11" s="7" t="s">
         <v>129</v>
       </c>
@@ -3253,7 +3458,7 @@
         <v>5.75</v>
       </c>
     </row>
-    <row r="12" spans="2:20" ht="25.5">
+    <row r="12" spans="2:20" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B12" s="7" t="s">
         <v>130</v>
       </c>
@@ -3278,7 +3483,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="13" spans="2:20" ht="25.5">
+    <row r="13" spans="2:20" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B13" s="7" t="s">
         <v>131</v>
       </c>
@@ -3303,7 +3508,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="2:20" ht="25.5">
+    <row r="14" spans="2:20" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B14" s="7" t="s">
         <v>132</v>
       </c>
@@ -3343,20 +3548,20 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="56.125" style="13" customWidth="1"/>
+    <col min="2" max="3" width="56.140625" style="13" customWidth="1"/>
     <col min="4" max="5" width="64" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="2:15" ht="27">
+    <row r="2" spans="2:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="s">
         <v>77</v>
       </c>
@@ -3366,7 +3571,7 @@
       <c r="F2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="2:15">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -3374,7 +3579,7 @@
       <c r="F3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="2:15" ht="25.5">
+    <row r="4" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
         <v>134</v>
       </c>
@@ -3386,7 +3591,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="25.5">
+    <row r="5" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B5" s="2" t="s">
         <v>88</v>
       </c>
@@ -3398,7 +3603,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="25.5">
+    <row r="6" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="1"/>
@@ -3408,7 +3613,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="25.5">
+    <row r="8" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B8" s="12" t="s">
         <v>12</v>
       </c>
@@ -3422,7 +3627,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="32.25">
+    <row r="9" spans="2:15" ht="33.75" x14ac:dyDescent="0.5">
       <c r="B9" s="9" t="s">
         <v>84</v>
       </c>
@@ -3441,7 +3646,7 @@
         <v>Produto CURSO Meia</v>
       </c>
     </row>
-    <row r="10" spans="2:15" ht="32.25">
+    <row r="10" spans="2:15" ht="33.75" x14ac:dyDescent="0.5">
       <c r="B10" s="9" t="s">
         <v>85</v>
       </c>
@@ -3460,7 +3665,7 @@
         <v>Meia Feminina Produto</v>
       </c>
     </row>
-    <row r="11" spans="2:15" ht="32.25">
+    <row r="11" spans="2:15" ht="33.75" x14ac:dyDescent="0.5">
       <c r="B11" s="9" t="s">
         <v>14</v>
       </c>
@@ -3477,7 +3682,7 @@
         <v>Camisa Masculina</v>
       </c>
     </row>
-    <row r="12" spans="2:15" ht="32.25">
+    <row r="12" spans="2:15" ht="33.75" x14ac:dyDescent="0.5">
       <c r="B12" s="9" t="s">
         <v>136</v>
       </c>
@@ -3494,7 +3699,7 @@
         <v>Bermuda Masculino CURSO</v>
       </c>
     </row>
-    <row r="13" spans="2:15" ht="32.25">
+    <row r="13" spans="2:15" ht="33.75" x14ac:dyDescent="0.5">
       <c r="B13" s="9" t="s">
         <v>16</v>
       </c>
@@ -3511,7 +3716,7 @@
         <v>Camisa Masculina Festa Balada</v>
       </c>
     </row>
-    <row r="14" spans="2:15" ht="32.25">
+    <row r="14" spans="2:15" ht="33.75" x14ac:dyDescent="0.5">
       <c r="B14" s="9" t="s">
         <v>86</v>
       </c>
@@ -3528,7 +3733,7 @@
         <v>Produto Jogger Meia</v>
       </c>
     </row>
-    <row r="15" spans="2:15" ht="32.25">
+    <row r="15" spans="2:15" ht="33.75" x14ac:dyDescent="0.5">
       <c r="B15" s="9" t="s">
         <v>17</v>
       </c>
@@ -3545,7 +3750,7 @@
         <v>Jaqueta Masculina Preta</v>
       </c>
     </row>
-    <row r="16" spans="2:15" ht="32.25">
+    <row r="16" spans="2:15" ht="33.75" x14ac:dyDescent="0.5">
       <c r="B16" s="9" t="s">
         <v>18</v>
       </c>
@@ -3562,7 +3767,7 @@
         <v>Bolsa de Trabalho</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="32.25">
+    <row r="17" spans="2:5" ht="33.75" x14ac:dyDescent="0.5">
       <c r="B17" s="9" t="s">
         <v>19</v>
       </c>
@@ -3594,25 +3799,25 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.5" style="13" customWidth="1"/>
-    <col min="8" max="8" width="55.125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="51.42578125" style="13" customWidth="1"/>
+    <col min="8" max="8" width="55.140625" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1"/>
       <c r="H1"/>
     </row>
-    <row r="2" spans="2:15" ht="27">
+    <row r="2" spans="2:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="s">
         <v>77</v>
       </c>
@@ -3622,7 +3827,7 @@
       <c r="G2"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="2:15">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="F3" s="1"/>
@@ -3632,7 +3837,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="25.5">
+    <row r="4" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
         <v>89</v>
       </c>
@@ -3646,7 +3851,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="25.5">
+    <row r="5" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="1"/>
@@ -3658,7 +3863,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="25.5">
+    <row r="6" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B6" s="3" t="s">
         <v>62</v>
       </c>
@@ -3681,7 +3886,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="30">
+    <row r="7" spans="2:15" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B7" s="7" t="s">
         <v>38</v>
       </c>
@@ -3716,7 +3921,7 @@
         <v xml:space="preserve">Tênis Feminino   </v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="30">
+    <row r="8" spans="2:15" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B8" s="7" t="s">
         <v>37</v>
       </c>
@@ -3753,7 +3958,7 @@
         <v xml:space="preserve">Calça Feminina Jogger  </v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="30">
+    <row r="9" spans="2:15" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B9" s="7" t="s">
         <v>39</v>
       </c>
@@ -3780,7 +3985,7 @@
         <v xml:space="preserve">Camisa Masculina   </v>
       </c>
     </row>
-    <row r="10" spans="2:15" ht="30">
+    <row r="10" spans="2:15" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B10" s="7" t="s">
         <v>41</v>
       </c>
@@ -3803,7 +4008,7 @@
         <v xml:space="preserve">Bermuda Masculino   </v>
       </c>
     </row>
-    <row r="11" spans="2:15" ht="30">
+    <row r="11" spans="2:15" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B11" s="7" t="s">
         <v>56</v>
       </c>
@@ -3830,7 +4035,7 @@
         <v xml:space="preserve">Camisa Masculina Festa Balada </v>
       </c>
     </row>
-    <row r="12" spans="2:15" ht="30">
+    <row r="12" spans="2:15" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B12" s="7" t="s">
         <v>42</v>
       </c>
@@ -3853,7 +4058,7 @@
         <v xml:space="preserve">Bota Masculina   </v>
       </c>
     </row>
-    <row r="13" spans="2:15" ht="30">
+    <row r="13" spans="2:15" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B13" s="7" t="s">
         <v>43</v>
       </c>
@@ -3878,7 +4083,7 @@
         <v xml:space="preserve">Jaqueta Masculina Preta  </v>
       </c>
     </row>
-    <row r="14" spans="2:15" ht="30">
+    <row r="14" spans="2:15" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B14" s="7" t="s">
         <v>45</v>
       </c>
@@ -3903,7 +4108,7 @@
         <v xml:space="preserve">Bolsa De Trabalho  </v>
       </c>
     </row>
-    <row r="15" spans="2:15" ht="30">
+    <row r="15" spans="2:15" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B15" s="7" t="s">
         <v>48</v>
       </c>
@@ -3946,34 +4151,34 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="57.5" customWidth="1"/>
-    <col min="3" max="3" width="22.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5" customWidth="1"/>
-    <col min="7" max="7" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E1"/>
       <c r="F1" s="1"/>
       <c r="H1"/>
     </row>
-    <row r="2" spans="2:15" ht="27">
+    <row r="2" spans="2:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="s">
         <v>77</v>
       </c>
       <c r="E2"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="2:15">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E3"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="2:15" ht="25.5">
+    <row r="4" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
         <v>90</v>
       </c>
@@ -3984,7 +4189,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="25.5">
+    <row r="5" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="F5" s="1"/>
@@ -3993,7 +4198,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="25.5">
+    <row r="6" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
@@ -4016,7 +4221,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="25.5">
+    <row r="7" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B7" s="4" t="s">
         <v>0</v>
       </c>
@@ -4043,7 +4248,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="25.5">
+    <row r="8" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B8" s="5" t="s">
         <v>1</v>
       </c>
@@ -4070,7 +4275,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="25.5">
+    <row r="9" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B9" s="5" t="s">
         <v>2</v>
       </c>
@@ -4094,7 +4299,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="2:15" ht="25.5">
+    <row r="10" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B10" s="5" t="s">
         <v>3</v>
       </c>
@@ -4118,7 +4323,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="2:15" ht="25.5">
+    <row r="11" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B11" s="5" t="s">
         <v>4</v>
       </c>
@@ -4139,7 +4344,7 @@
         <v>hotmail</v>
       </c>
     </row>
-    <row r="12" spans="2:15" ht="25.5">
+    <row r="12" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B12" s="5" t="s">
         <v>5</v>
       </c>
@@ -4183,21 +4388,21 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="57.5" customWidth="1"/>
-    <col min="3" max="3" width="22.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.75" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F1" s="1"/>
       <c r="G1"/>
     </row>
-    <row r="2" spans="2:15" ht="27">
+    <row r="2" spans="2:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="s">
         <v>77</v>
       </c>
@@ -4205,7 +4410,7 @@
       <c r="G2"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="2:15">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F3" s="1"/>
       <c r="G3"/>
       <c r="H3" s="1"/>
@@ -4213,7 +4418,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="25.5">
+    <row r="4" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
         <v>99</v>
       </c>
@@ -4225,7 +4430,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="19.5" customHeight="1">
+    <row r="5" spans="2:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="E5" s="1"/>
@@ -4235,7 +4440,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="25.5">
+    <row r="6" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -4255,7 +4460,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="25.5">
+    <row r="7" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
@@ -4276,7 +4481,7 @@
       <c r="I7" s="1"/>
       <c r="O7" s="21"/>
     </row>
-    <row r="8" spans="2:15" ht="25.5">
+    <row r="8" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B8" s="7" t="s">
         <v>69</v>
       </c>
@@ -4296,7 +4501,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="2:15" ht="25.5">
+    <row r="9" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B9" s="7" t="s">
         <v>70</v>
       </c>
@@ -4326,25 +4531,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P16"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="57.5" customWidth="1"/>
-    <col min="3" max="3" width="22.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="40.25" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.5" customWidth="1"/>
-    <col min="7" max="7" width="33.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="57.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.42578125" customWidth="1"/>
+    <col min="7" max="7" width="33.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
       <c r="F1" s="1"/>
       <c r="G1"/>
     </row>
-    <row r="2" spans="2:16" ht="27">
+    <row r="2" spans="2:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="s">
         <v>77</v>
       </c>
@@ -4352,7 +4557,7 @@
       <c r="G2"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="2:16">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="F3" s="1"/>
       <c r="G3"/>
       <c r="H3" s="1"/>
@@ -4360,7 +4565,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="25.5">
+    <row r="4" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
         <v>100</v>
       </c>
@@ -4372,7 +4577,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="2:16" ht="25.5">
+    <row r="5" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B5" s="2" t="s">
         <v>101</v>
       </c>
@@ -4384,7 +4589,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="2:16" ht="19.5" customHeight="1">
+    <row r="6" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="E6" s="1"/>
@@ -4394,7 +4599,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="25.5">
+    <row r="7" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
@@ -4419,7 +4624,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="2:16" ht="25.5">
+    <row r="8" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B8" s="7" t="s">
         <v>71</v>
       </c>
@@ -4449,7 +4654,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="25.5">
+    <row r="9" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B9" s="7" t="s">
         <v>72</v>
       </c>
@@ -4477,17 +4682,17 @@
       <c r="I9" s="1"/>
       <c r="P9" s="21"/>
     </row>
-    <row r="10" spans="2:16">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="P10" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="2:16" ht="25.5">
+    <row r="11" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="P11" s="21" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="2:16" ht="25.5">
+    <row r="12" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="H12" s="1"/>
@@ -4495,7 +4700,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="2:16" ht="25.5">
+    <row r="13" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B13" s="3" t="s">
         <v>9</v>
       </c>
@@ -4511,7 +4716,7 @@
       <c r="F13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="2:16" ht="25.5">
+    <row r="14" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B14" s="7" t="s">
         <v>71</v>
       </c>
@@ -4532,7 +4737,7 @@
       <c r="F14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="2:16" ht="25.5">
+    <row r="15" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B15" s="7" t="s">
         <v>72</v>
       </c>
@@ -4553,7 +4758,7 @@
       <c r="F15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="2:16">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="H16" s="1"/>
@@ -4572,25 +4777,25 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="52.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.75" style="1"/>
-    <col min="5" max="5" width="52.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="1"/>
+    <col min="5" max="5" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="27">
+    <row r="2" spans="2:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="s">
         <v>77</v>
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="2:16">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="2:16" ht="25.5">
+    <row r="4" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
         <v>76</v>
       </c>
@@ -4600,7 +4805,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="2:16" ht="25.5">
+    <row r="5" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B5" s="2" t="s">
         <v>82</v>
       </c>
@@ -4610,17 +4815,17 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="2:16" ht="25.5">
+    <row r="6" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B6" s="2"/>
       <c r="E6" s="2"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="2:16" ht="25.5">
+    <row r="7" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B7" s="2"/>
       <c r="E7" s="2"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="2:16" ht="19.5">
+    <row r="8" spans="2:16" ht="21" x14ac:dyDescent="0.35">
       <c r="B8" s="15" t="s">
         <v>74</v>
       </c>
@@ -4632,7 +4837,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="2:16" ht="25.5">
+    <row r="9" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
@@ -4646,7 +4851,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:16" ht="25.5">
+    <row r="10" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B10" s="7" t="s">
         <v>20</v>
       </c>
@@ -4662,7 +4867,7 @@
         <v>89.99</v>
       </c>
     </row>
-    <row r="11" spans="2:16" ht="25.5">
+    <row r="11" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B11" s="7" t="s">
         <v>21</v>
       </c>
@@ -4678,7 +4883,7 @@
         <v>69.989999999999995</v>
       </c>
     </row>
-    <row r="12" spans="2:16" ht="25.5">
+    <row r="12" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B12" s="7" t="s">
         <v>27</v>
       </c>
@@ -4694,7 +4899,7 @@
         <v>153.4</v>
       </c>
     </row>
-    <row r="13" spans="2:16" ht="25.5">
+    <row r="13" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B13" s="7" t="s">
         <v>22</v>
       </c>
@@ -4710,7 +4915,7 @@
         <v>148.56</v>
       </c>
     </row>
-    <row r="14" spans="2:16" ht="25.5">
+    <row r="14" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B14" s="7" t="s">
         <v>23</v>
       </c>
@@ -4726,7 +4931,7 @@
         <v>146.13999999999999</v>
       </c>
     </row>
-    <row r="15" spans="2:16" ht="25.5">
+    <row r="15" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B15" s="7" t="s">
         <v>24</v>
       </c>
@@ -4742,7 +4947,7 @@
         <v>224.14</v>
       </c>
     </row>
-    <row r="16" spans="2:16" ht="25.5">
+    <row r="16" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B16" s="7" t="s">
         <v>25</v>
       </c>
@@ -4758,7 +4963,7 @@
         <v>150.5</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="25.5">
+    <row r="17" spans="2:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B17" s="7" t="s">
         <v>26</v>
       </c>

</xml_diff>